<commit_message>
libellé rum ano 19
</commit_message>
<xml_diff>
--- a/formats/excel/Formats RUM 19.xlsx
+++ b/formats/excel/Formats RUM 19.xlsx
@@ -312,6 +312,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -388,8 +389,8 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>